<commit_message>
30, 31 ques done . 2D started .
</commit_message>
<xml_diff>
--- a/out/production/complete_DS-ALGO_In_450Questions/quesSheet/FINAL450.xlsx
+++ b/out/production/complete_DS-ALGO_In_450Questions/quesSheet/FINAL450.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IntellijProjects\leetcodepractice\src\quesSheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IntellijProjects\leetcodepractice\out\production\complete_DS-ALGO_In_450Questions\quesSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B584B0CC-AC0A-4002-AA71-F2B2BF7E3CC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D39B552D-7ADB-424C-AB0A-1DB37DB276B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1863,8 +1863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2238,7 +2238,7 @@
         <v>36</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="21">

</xml_diff>